<commit_message>
made adjustments based on eb requests
</commit_message>
<xml_diff>
--- a/templates/flow_template.xlsx
+++ b/templates/flow_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nickl\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sccwrp.sharepoint.com/sites/Staff/Shared Documents/P Drive/Data/DuyNguyen/Projects/rainfall_flow_calculator_shiny/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0F45A3E-2991-4552-98CD-6C047B03EB08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{F0F45A3E-2991-4552-98CD-6C047B03EB08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{63716E53-84C9-4C6A-9915-75AB1084B0C7}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -120,13 +120,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>19051</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>304799</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -141,8 +141,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="19050"/>
-          <a:ext cx="8229599" cy="9772650"/>
+          <a:off x="0" y="19051"/>
+          <a:ext cx="8229599" cy="5981700"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -177,201 +177,183 @@
         <a:lstStyle/>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
             <a:t>Application Usage Guide</a:t>
           </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
             <a:t>=======================</a:t>
           </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
             <a:t>This guide provides instructions for using the application and outlines the data requirements for successful analysis.</a:t>
           </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
             <a:t>Analysis Types</a:t>
           </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
             <a:t>--------------</a:t>
           </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
             <a:t>IMPORTANT: The column names and tab names in the templates (both rainfall and flow) must remain unchanged for accurate analysis and app's functionality.</a:t>
           </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>The application supports two types of analysis: Rainfall Analysis and Flow Analysis.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>The application supports two types of analysis: Rainfall Analysis and Flow Analysis. </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>---------------------</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
             <a:t>Rainfall Analysis</a:t>
           </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>-----------------</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>To perform a Rainfall Analysis, follow these steps:</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>1. Open the rainfall template (rainfall_template.xlsx).</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>2. Copy and paste the rainfall data into the template.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>3. Ensure that the rain gauge values are entered into the designated rain column within the template.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Demo data is provided</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> on the instructions tab of the application</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Flow Analysis</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>-------------</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>To perform a Flow Analysis, follow these steps:</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>1. Open the flow template (flow_template.xlsx).</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>2. Copy and paste the flow data from your datasheet into the downloaded template.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>3. Accommodate up to four flows for analysis: inflow 1, inflow 2, outflow, and bypass.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>4. Refer to the Methods tab in the template for an illustration of the possible flow type configurations.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>5. You are not required to submit data for all four flow types; any combination of flow types is acceptable.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>IMPORTANT: If any of the flow data types are not applicable, leave the corresponding tab blank. Do not modify the column names or the tab names.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Demo data is provided</a:t>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>: The user is advised to copy and paste the rainfall data, whether it is in the form of 1-minute or time-of-tips data, into the downloaded template. It is important to note that the rain gauge values must be entered into the designated rain column within the template. Continuous rainfall data are submittable.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Demo data are available on the Shin</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0">
@@ -383,95 +365,277 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> on the instructions tab of the application</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>.</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>y App.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>---------------------</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Flow</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> Analysis</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>: Flow data should be copy-pasted from the user's datasheet to the downloaded data template. Up to four flows can be accomodated for analysis. The available flow types are inflow 1, inflow 2, outflow and bypass. Refer to the Methods tab for an illustration of the possible flow type configurations. A user does not need to submit all four types, any combination of the flow types is acceptable. A user can only submit flow data for a single rain event. If any of the data types are not applicable, leave the tab blank (as is)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Demo data are available on the Shin</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>y App.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>---------------------</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
             <a:t>Data Requirements</a:t>
           </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>-----------------</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>---------------------</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
             <a:t>To ensure successful analysis, the uploaded Excel spreadsheet must conform to the following requirements:</a:t>
           </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
             <a:t>- Flow must be reported in units of L/s, gpm, or cfs.</a:t>
           </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
             <a:t>- The timestamp should be in 24-hour format (mm/dd/yy hh:mm:ss).</a:t>
           </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
             <a:t>- Each tab must contain exactly two columns: one for the sample timestamps data and one for the associated values.</a:t>
           </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
             <a:t>- The column names and the tab names must not be changed from the template.</a:t>
           </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
             <a:t>Please ensure that your data meets these requirements before using the application for analysis.</a:t>
           </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
             <a:t>For further assistance or inquiries, please contact our support team at stormwater@sccwrp.org</a:t>
           </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:endParaRPr lang="en-US" sz="1100"/>
@@ -749,7 +913,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P32" sqref="P32"/>
+      <selection activeCell="R20" sqref="R20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -869,6 +1033,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -881,9 +1054,9 @@
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000C0FD75001275F4DBA43EB7BE58C8A34" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="21cacd0d90dbd8beb6fc12ad84d4cd0e">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="02ea596c-bf3f-4512-ad68-024a720c79b2" xmlns:ns3="959569b2-1f16-4dd0-b5ed-bb064e5cd07e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5b418c8325abc32123734ac979891270" ns1:_="" ns2:_="" ns3:_="">
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000C0FD75001275F4DBA43EB7BE58C8A34" ma:contentTypeVersion="20" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="582b150a9eb9a8984bd6398cf909f49d">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="02ea596c-bf3f-4512-ad68-024a720c79b2" xmlns:ns3="959569b2-1f16-4dd0-b5ed-bb064e5cd07e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a4808acce3a6e68b39fbd804e31fb38" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
     <xsd:import namespace="02ea596c-bf3f-4512-ad68-024a720c79b2"/>
     <xsd:import namespace="959569b2-1f16-4dd0-b5ed-bb064e5cd07e"/>
@@ -910,6 +1083,7 @@
                 <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyProperties" minOccurs="0"/>
                 <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyUIAction" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -998,6 +1172,11 @@
     <xsd:element name="MediaServiceSearchProperties" ma:index="25" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="26" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:description="" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -1141,16 +1320,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{30E79D0C-F610-4EAE-A025-AE59D3D7877F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC2A99C6-72A4-4F0E-BB64-9F38352613FB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -1162,8 +1340,8 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03F51464-0A33-49BF-B995-F3FF88D35341}">
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EFD43180-1C57-4BDF-BF67-33B122A932DF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
@@ -1180,12 +1358,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{30E79D0C-F610-4EAE-A025-AE59D3D7877F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>